<commit_message>
Arquivos da Semana da PÓS e Revisão da Proposta
</commit_message>
<xml_diff>
--- a/10-planejamento/cronograma/cronograma.xlsx
+++ b/10-planejamento/cronograma/cronograma.xlsx
@@ -5,17 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>CRONOGRAMA DISSERTAÇÃO</t>
   </si>
@@ -32,52 +37,70 @@
     <t>Término (MM/AAAA)</t>
   </si>
   <si>
-    <t>Revisão Sistemática da Literatura</t>
+    <t>Mapeamento  Sistemático da Literatura</t>
+  </si>
+  <si>
+    <t>03/2016</t>
+  </si>
+  <si>
+    <t>06/2016</t>
+  </si>
+  <si>
+    <t>Ponto de Controle 01 – Reunião com orientador sobre Revisão Sistemática da Literatura</t>
+  </si>
+  <si>
+    <t>Caracterização das Ferramentas de Gerenciamento de Requisição de Mudança</t>
+  </si>
+  <si>
+    <t>07/2016</t>
+  </si>
+  <si>
+    <t>Ponto de Controle 02 – Reunião com orientador sobre a Caracterizão das FGRM</t>
+  </si>
+  <si>
+    <t>Pesquisa com Profissionais</t>
+  </si>
+  <si>
+    <t>08/2016</t>
+  </si>
+  <si>
+    <t>09/2016</t>
+  </si>
+  <si>
+    <t>Ponto de Controle 03 – Reunião com orientador sobre a Pesquisa com o Profissionais</t>
+  </si>
+  <si>
+    <t>Implementação da Ferramenta</t>
+  </si>
+  <si>
+    <t>10/2016</t>
+  </si>
+  <si>
+    <t>Ponto de Controle 03 – Avaliação da Ferramenta Avaliada</t>
+  </si>
+  <si>
+    <t>Experimento de Avaliação da Ferramenta</t>
+  </si>
+  <si>
+    <t>11/2016</t>
+  </si>
+  <si>
+    <t>Ponto de Controle 04 – Avaliação do Experimento junto com o orientador</t>
+  </si>
+  <si>
+    <t>Finalização do texto da dissertação</t>
+  </si>
+  <si>
+    <t>12/2017</t>
   </si>
   <si>
     <t>12/2016</t>
   </si>
   <si>
-    <t>02/2016</t>
-  </si>
-  <si>
-    <t>Ponto de Controle 01 – Reunião com orientador sobre Revisão Sistemática da Literatura</t>
-  </si>
-  <si>
-    <t>Pesquisa com Profissionais</t>
-  </si>
-  <si>
-    <t>04/2016</t>
-  </si>
-  <si>
-    <t>Ponto de Controle 02 – Reunião com orientador sobre a Pesquisa com o Profissionais</t>
-  </si>
-  <si>
-    <t>Implementação da Ferramenta</t>
-  </si>
-  <si>
-    <t>06/2016</t>
-  </si>
-  <si>
-    <t>Ponto de Controle 03 – Avaliação da Ferramenta Avaliada</t>
-  </si>
-  <si>
-    <t>Experimento de Avaliação da Ferramenta</t>
-  </si>
-  <si>
-    <t>07/2016</t>
-  </si>
-  <si>
-    <t>Ponto de Controle 04 – Avaliação do Experimento junto com o orientador</t>
-  </si>
-  <si>
-    <t>Finalização do texto da dissertação</t>
-  </si>
-  <si>
-    <t>08/2016</t>
-  </si>
-  <si>
     <t>Ponto de Controle 05 – Avaliação do texto da dissertação com o orientador</t>
+  </si>
+  <si>
+    <t>01/2017</t>
   </si>
   <si>
     <t>Defesa da dissertação</t>
@@ -233,19 +256,19 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.55612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="65.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
@@ -284,7 +307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
@@ -298,7 +321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
@@ -312,7 +335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
@@ -326,7 +349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
@@ -334,94 +357,122 @@
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>